<commit_message>
Calcul of surface by bulding cathegory
</commit_message>
<xml_diff>
--- a/Trey/DATA/mini-projet-trey/input-data/trey_power_network.xlsx
+++ b/Trey/DATA/mini-projet-trey/input-data/trey_power_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thierryfra\github\perso\rhtlab_test_labo\Trey\DATA\mini-projet-trey\input-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E55818-18B4-4DF0-B88D-77561F62B558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D50CE-A774-49CE-8600-0AD6F4C57B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -318,9 +318,6 @@
     <t>GKN3X240_240</t>
   </si>
   <si>
-    <t>N60437</t>
-  </si>
-  <si>
     <t>ext_grid_0</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
   </si>
   <si>
     <t>Trafo</t>
+  </si>
+  <si>
+    <t>60437</t>
   </si>
 </sst>
 </file>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD154A9-14F2-4509-A0AA-B0D37BD7BC37}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,7 +800,7 @@
         <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -817,7 +817,7 @@
         <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -834,7 +834,7 @@
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -851,7 +851,7 @@
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -868,7 +868,7 @@
         <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -936,7 +936,7 @@
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -953,7 +953,7 @@
         <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -970,15 +970,15 @@
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>92</v>
+      <c r="B13" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C13">
         <v>0.4</v>
@@ -987,7 +987,7 @@
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Calcul power for each cabinet
</commit_message>
<xml_diff>
--- a/Trey/DATA/mini-projet-trey/input-data/trey_power_network.xlsx
+++ b/Trey/DATA/mini-projet-trey/input-data/trey_power_network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thierryfra\github\perso\rhtlab_test_labo\Trey\DATA\mini-projet-trey\input-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D50CE-A774-49CE-8600-0AD6F4C57B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBF6FB7-F3A8-4F2B-BC93-0DFDA37107F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{5FC146A3-AC37-46DC-AD92-E888F69598AC}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>60437</t>
+  </si>
+  <si>
+    <t>STMT003438HV</t>
   </si>
 </sst>
 </file>
@@ -757,13 +760,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD154A9-14F2-4509-A0AA-B0D37BD7BC37}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,10 +798,10 @@
         <v>68</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>0.4</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
         <v>95</v>
@@ -993,6 +997,18 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1096,7 +1112,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,7 +1820,7 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,6 +1929,36 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.63</v>
+      </c>
+      <c r="F2">
+        <v>18.3</v>
+      </c>
+      <c r="G2">
+        <v>0.42</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>0.42</v>
+      </c>
+      <c r="J2">
+        <v>0.65</v>
+      </c>
+      <c r="K2">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2074,7 +2120,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2134,7 +2180,7 @@
         <v>92</v>
       </c>
       <c r="C2" s="7">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2534,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB91AA0C-6E10-4C2C-B831-A2E20673E5F8}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2588,60 +2634,168 @@
       <c r="A2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2.2329000000000002E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4.1394E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>9.188E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2.2412999999999999E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>6.8910000000000004E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>6.352E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>4.3998000000000002E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1.0565E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>6.4539999999999997E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>2.5128999999999999E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>9.5980000000000006E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>1.0946000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>